<commit_message>
python script now generates mealplan in text file
</commit_message>
<xml_diff>
--- a/meals.xlsx
+++ b/meals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mayaf\Documents\Projects\coding\python\meal_planner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E6CB13-AFDB-4AA8-BA11-D72FF797E2B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7DD62F5-9150-4F07-AA01-C328FC6ED2EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
   <si>
     <t>recipe_name</t>
   </si>
@@ -60,9 +60,6 @@
     <t>baked salmon and veggies</t>
   </si>
   <si>
-    <t>salmon</t>
-  </si>
-  <si>
     <t>paprika, carrot, potato, onion</t>
   </si>
   <si>
@@ -114,9 +111,6 @@
     <t>carrot, potato</t>
   </si>
   <si>
-    <t>pineapple</t>
-  </si>
-  <si>
     <t>fiskeboller, potato, carrots</t>
   </si>
   <si>
@@ -126,16 +120,52 @@
     <t>kjøttboller, fløtesaus, tyttebær</t>
   </si>
   <si>
-    <t>mango chutney, rice</t>
-  </si>
-  <si>
     <t>potato</t>
   </si>
   <si>
-    <t xml:space="preserve">milk </t>
-  </si>
-  <si>
     <t>paella</t>
+  </si>
+  <si>
+    <t>canned tomato, beans</t>
+  </si>
+  <si>
+    <t>carrot, spring onion</t>
+  </si>
+  <si>
+    <t>burgers, fries</t>
+  </si>
+  <si>
+    <t>flour, egg, milk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">milk, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">pasta, </t>
+  </si>
+  <si>
+    <t>salmon,</t>
+  </si>
+  <si>
+    <t>pineapple,</t>
+  </si>
+  <si>
+    <t>fish, fries,</t>
+  </si>
+  <si>
+    <t>rice, fish, veg,</t>
+  </si>
+  <si>
+    <t>mango chutney, rice,</t>
+  </si>
+  <si>
+    <t>noodles,</t>
+  </si>
+  <si>
+    <t>miso, dashi, noodles,</t>
+  </si>
+  <si>
+    <t>couscous, aubergine,</t>
   </si>
 </sst>
 </file>
@@ -179,7 +209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -187,19 +217,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -485,57 +503,57 @@
   <dimension ref="A1:AP18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="4"/>
-    <col min="2" max="2" width="16.5703125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="15" style="4" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" style="7"/>
-    <col min="8" max="8" width="6.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.42578125" style="7"/>
-    <col min="14" max="14" width="6.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.42578125" style="7"/>
-    <col min="20" max="20" width="6.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16.42578125" style="7"/>
-    <col min="26" max="26" width="6.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="8.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="5.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.42578125" style="7"/>
-    <col min="32" max="32" width="6.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="8.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="10.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="5.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="16.42578125" style="7"/>
-    <col min="38" max="38" width="6.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="8.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="6.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="10.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="5.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="43" max="16384" width="16.42578125" style="4"/>
+    <col min="1" max="1" width="16.44140625" style="3"/>
+    <col min="2" max="2" width="16.5546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="15" style="3" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.44140625" style="3"/>
+    <col min="8" max="8" width="6.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.44140625" style="3"/>
+    <col min="14" max="14" width="6.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.44140625" style="3"/>
+    <col min="20" max="20" width="6.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.44140625" style="3"/>
+    <col min="26" max="26" width="6.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="5.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.44140625" style="3"/>
+    <col min="32" max="32" width="6.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="6.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="5.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="16.44140625" style="3"/>
+    <col min="38" max="38" width="6.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="6.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="10.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="5.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="43" max="16384" width="16.44140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -550,215 +568,237 @@
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="5"/>
-      <c r="AB1" s="5"/>
-      <c r="AC1" s="5"/>
-      <c r="AD1" s="5"/>
-      <c r="AE1" s="6"/>
-      <c r="AF1" s="5"/>
-      <c r="AG1" s="5"/>
-      <c r="AH1" s="5"/>
-      <c r="AI1" s="5"/>
-      <c r="AJ1" s="5"/>
-      <c r="AK1" s="6"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
+      <c r="AF1" s="1"/>
+      <c r="AG1" s="1"/>
+      <c r="AH1" s="1"/>
+      <c r="AI1" s="1"/>
+      <c r="AJ1" s="1"/>
       <c r="AL1" s="1"/>
       <c r="AM1" s="1"/>
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
     </row>
-    <row r="2" spans="1:42" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    </row>
+    <row r="3" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:42" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="C7" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:42" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="C8" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:42" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:42" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="4" t="s">
+      <c r="B11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="4" t="s">
+    <row r="13" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="B15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:42" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+    <row r="16" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="B16" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="D16" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="B17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="4" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
now adds shopping list
</commit_message>
<xml_diff>
--- a/meals.xlsx
+++ b/meals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mayaf\Documents\Projects\coding\python\meal_planner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7DD62F5-9150-4F07-AA01-C328FC6ED2EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449CAF84-3496-4DF3-9B13-51273541E30C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,21 +48,12 @@
     <t>curry</t>
   </si>
   <si>
-    <t>rice, coconut milk</t>
-  </si>
-  <si>
     <t>fresh_ingredients</t>
   </si>
   <si>
-    <t>carrot</t>
-  </si>
-  <si>
     <t>baked salmon and veggies</t>
   </si>
   <si>
-    <t>paprika, carrot, potato, onion</t>
-  </si>
-  <si>
     <t>nachos</t>
   </si>
   <si>
@@ -108,36 +99,18 @@
     <t>fish with fries</t>
   </si>
   <si>
-    <t>carrot, potato</t>
-  </si>
-  <si>
-    <t>fiskeboller, potato, carrots</t>
-  </si>
-  <si>
     <t>chicken, cheese, wraps, taco herbs</t>
   </si>
   <si>
     <t>kjøttboller, fløtesaus, tyttebær</t>
   </si>
   <si>
-    <t>potato</t>
-  </si>
-  <si>
     <t>paella</t>
   </si>
   <si>
     <t>canned tomato, beans</t>
   </si>
   <si>
-    <t>carrot, spring onion</t>
-  </si>
-  <si>
-    <t>burgers, fries</t>
-  </si>
-  <si>
-    <t>flour, egg, milk</t>
-  </si>
-  <si>
     <t xml:space="preserve">milk, </t>
   </si>
   <si>
@@ -166,6 +139,33 @@
   </si>
   <si>
     <t>couscous, aubergine,</t>
+  </si>
+  <si>
+    <t>rice, coconut milk,</t>
+  </si>
+  <si>
+    <t>burgers, fries,</t>
+  </si>
+  <si>
+    <t>flour, egg, milk,</t>
+  </si>
+  <si>
+    <t>fiskeboller, potato, carrots,</t>
+  </si>
+  <si>
+    <t>paprika, carrot, potato, onion,</t>
+  </si>
+  <si>
+    <t>carrot, potato,</t>
+  </si>
+  <si>
+    <t>potato,</t>
+  </si>
+  <si>
+    <t>carrot,</t>
+  </si>
+  <si>
+    <t>carrot, spring onion,</t>
   </si>
 </sst>
 </file>
@@ -502,8 +502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -564,7 +564,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -602,110 +602,110 @@
     </row>
     <row r="2" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:42" x14ac:dyDescent="0.3">
@@ -713,7 +713,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>4</v>
@@ -724,21 +724,21 @@
         <v>5</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>4</v>
@@ -746,10 +746,10 @@
     </row>
     <row r="14" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>4</v>
@@ -757,10 +757,10 @@
     </row>
     <row r="15" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>4</v>
@@ -768,24 +768,24 @@
     </row>
     <row r="16" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>4</v>
@@ -793,10 +793,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
added a quit button to ui
</commit_message>
<xml_diff>
--- a/meals.xlsx
+++ b/meals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mayaf\Documents\Projects\coding\python\meal_planner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D999FDB2-ACAF-49E7-B56D-DC0BAECAC2EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8952631A-4C32-4A7B-A984-CA85D58E6969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -503,7 +503,7 @@
   <dimension ref="A1:AP18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
cleaned up code, added function to add recipe to dataframe
</commit_message>
<xml_diff>
--- a/meals.xlsx
+++ b/meals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mayaf\Documents\Projects\coding\python\meal_planner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8952631A-4C32-4A7B-A984-CA85D58E6969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3795FBC-AD5A-4694-890D-3EE3EF57262B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
   <si>
     <t>recipe_name</t>
   </si>
@@ -166,6 +166,18 @@
   </si>
   <si>
     <t>carrot, spring_onion,</t>
+  </si>
+  <si>
+    <t>chicken_wings</t>
+  </si>
+  <si>
+    <t>instructions</t>
+  </si>
+  <si>
+    <t>add anything that is leftover</t>
+  </si>
+  <si>
+    <t>leftovers</t>
   </si>
 </sst>
 </file>
@@ -500,10 +512,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AP18"/>
+  <dimension ref="A1:AP19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -566,7 +579,9 @@
       <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1"/>
+      <c r="E1" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -616,129 +631,126 @@
     </row>
     <row r="3" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:42" ht="43.2" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:42" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>4</v>
@@ -746,66 +758,86 @@
     </row>
     <row r="14" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:42" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E16" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E17" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>4</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:D18" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D18">
-      <sortCondition ref="C1:C18"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D19">
+      <sortCondition ref="A1:A18"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed bug where shopping list got shuffled
</commit_message>
<xml_diff>
--- a/meals.xlsx
+++ b/meals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mayaf\Documents\Projects\coding\python\meal_planner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3795FBC-AD5A-4694-890D-3EE3EF57262B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A16D1E5-44B3-44EB-8194-8C5E179BC276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="51">
   <si>
     <t>recipe_name</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>leftovers</t>
+  </si>
+  <si>
+    <t>chicken_wings,</t>
   </si>
 </sst>
 </file>
@@ -515,8 +518,8 @@
   <dimension ref="A1:AP19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -667,7 +670,7 @@
         <v>46</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>19</v>

</xml_diff>